<commit_message>
Aggiunti test LAB_TRASF mancanti, fix stringhe nella colonna "Razionale" della checklist
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.56/report-checklist.xlsx
+++ b/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.56/report-checklist.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="33720" yWindow="975" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Istruzioni Compilazione" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Prerequisiti" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TestCases" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="LISTA VALORI" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="Summary" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Istruzioni Compilazione" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Prerequisiti" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestCases" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LISTA VALORI" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'TestCases'!$A$9:$W$192</definedName>
@@ -2249,7 +2249,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W602"/>
+  <dimension ref="A1:W604"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
@@ -2627,22 +2627,22 @@
       </c>
       <c r="F10" s="66" t="inlineStr">
         <is>
-          <t>2025-11-10</t>
+          <t>2025-11-12</t>
         </is>
       </c>
       <c r="G10" s="66" t="inlineStr">
         <is>
-          <t>2025-11-10T12:04:09Z</t>
+          <t>2025-11-12T12:59:27Z</t>
         </is>
       </c>
       <c r="H10" s="66" t="inlineStr">
         <is>
-          <t>e134f5a6cfbcb423c1c0dffb37b40c18</t>
+          <t>252fba4d949e5beb5a6baa1f9df9e407</t>
         </is>
       </c>
       <c r="I10" s="67" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.c6a644fd170a5de765b2a481be6f0222350fec99717fc407eeda72f58d67f90b.75a924ebe2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.91183dba9faaea11a6d674223c8b24d2a6b93c804b899ca0eb4b8d4bcdf5532c.c4c6e65889^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J10" s="68" t="inlineStr">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="K11" s="73" t="inlineStr">
         <is>
-          <t>l'applicativo effettua controlli preventivi sul dato inserito</t>
+          <t>L'applicativo effettua controlli preventivi sul dato inserito</t>
         </is>
       </c>
       <c r="L11" s="73" t="n"/>
@@ -2722,11 +2722,7 @@
       <c r="Q11" s="73" t="n"/>
       <c r="R11" s="73" t="n"/>
       <c r="S11" s="73" t="n"/>
-      <c r="T11" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T11" s="73" t="inlineStr"/>
       <c r="U11" s="74" t="n"/>
       <c r="V11" s="75" t="n"/>
       <c r="W11" s="73" t="inlineStr">
@@ -2774,7 +2770,7 @@
       </c>
       <c r="K12" s="73" t="inlineStr">
         <is>
-          <t>l'applicativo effettua controlli preventivi sul dato inserito</t>
+          <t>L'applicativo effettua controlli preventivi sul dato inserito</t>
         </is>
       </c>
       <c r="L12" s="73" t="n"/>
@@ -2785,11 +2781,7 @@
       <c r="Q12" s="73" t="n"/>
       <c r="R12" s="73" t="n"/>
       <c r="S12" s="73" t="n"/>
-      <c r="T12" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T12" s="73" t="inlineStr"/>
       <c r="U12" s="74" t="n"/>
       <c r="V12" s="75" t="n"/>
       <c r="W12" s="73" t="inlineStr">
@@ -2837,7 +2829,7 @@
       </c>
       <c r="K13" s="73" t="inlineStr">
         <is>
-          <t>l'applicativo effettua controlli preventivi sul dato inserito</t>
+          <t>L'applicativo effettua controlli preventivi sul dato inserito</t>
         </is>
       </c>
       <c r="L13" s="73" t="n"/>
@@ -2848,11 +2840,7 @@
       <c r="Q13" s="73" t="n"/>
       <c r="R13" s="73" t="n"/>
       <c r="S13" s="73" t="n"/>
-      <c r="T13" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T13" s="73" t="inlineStr"/>
       <c r="U13" s="74" t="n"/>
       <c r="V13" s="75" t="n"/>
       <c r="W13" s="73" t="inlineStr">
@@ -2900,7 +2888,7 @@
       </c>
       <c r="K14" s="73" t="inlineStr">
         <is>
-          <t>l'applicativo effettua controlli preventivi sul dato inserito</t>
+          <t>L'applicativo effettua controlli preventivi sul dato inserito</t>
         </is>
       </c>
       <c r="L14" s="73" t="n"/>
@@ -2911,11 +2899,7 @@
       <c r="Q14" s="73" t="n"/>
       <c r="R14" s="73" t="n"/>
       <c r="S14" s="73" t="n"/>
-      <c r="T14" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T14" s="73" t="inlineStr"/>
       <c r="U14" s="74" t="n"/>
       <c r="V14" s="75" t="n"/>
       <c r="W14" s="73" t="inlineStr">
@@ -2951,12 +2935,12 @@
       </c>
       <c r="F15" s="76" t="inlineStr">
         <is>
-          <t>2025-11-10</t>
+          <t>2025-11-12</t>
         </is>
       </c>
       <c r="G15" s="76" t="inlineStr">
         <is>
-          <t>2025-11-10T12:44:06Z</t>
+          <t>2025-11-12T13:00:35Z</t>
         </is>
       </c>
       <c r="H15" s="76" t="inlineStr">
@@ -3051,12 +3035,12 @@
       </c>
       <c r="F16" s="76" t="inlineStr">
         <is>
-          <t>2025-11-10</t>
+          <t>2025-11-12</t>
         </is>
       </c>
       <c r="G16" s="76" t="inlineStr">
         <is>
-          <t>2025-11-10T12:44:06Z</t>
+          <t>2025-11-12T13:00:35Z</t>
         </is>
       </c>
       <c r="H16" s="76" t="inlineStr">
@@ -3160,7 +3144,7 @@
       </c>
       <c r="K17" s="73" t="inlineStr">
         <is>
-          <t>l'applicativo effettua controlli preventivi sul dato inserito</t>
+          <t>L'applicativo effettua controlli preventivi sul dato inserito</t>
         </is>
       </c>
       <c r="L17" s="73" t="n"/>
@@ -3171,11 +3155,7 @@
       <c r="Q17" s="73" t="n"/>
       <c r="R17" s="73" t="n"/>
       <c r="S17" s="73" t="n"/>
-      <c r="T17" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T17" s="73" t="inlineStr"/>
       <c r="U17" s="74" t="n"/>
       <c r="V17" s="75" t="n"/>
       <c r="W17" s="73" t="inlineStr">
@@ -3220,7 +3200,7 @@
       </c>
       <c r="K18" s="73" t="inlineStr">
         <is>
-          <t>campo obbligatorio</t>
+          <t>Campo obbligatorio</t>
         </is>
       </c>
       <c r="L18" s="73" t="n"/>
@@ -3231,11 +3211,7 @@
       <c r="Q18" s="73" t="n"/>
       <c r="R18" s="73" t="n"/>
       <c r="S18" s="73" t="n"/>
-      <c r="T18" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T18" s="73" t="inlineStr"/>
       <c r="U18" s="74" t="n"/>
       <c r="V18" s="75" t="n"/>
       <c r="W18" s="73" t="inlineStr">
@@ -3280,7 +3256,7 @@
       </c>
       <c r="K19" s="73" t="inlineStr">
         <is>
-          <t>campo obbligatorio</t>
+          <t>Campo obbligatorio</t>
         </is>
       </c>
       <c r="L19" s="73" t="n"/>
@@ -3291,11 +3267,7 @@
       <c r="Q19" s="73" t="n"/>
       <c r="R19" s="73" t="n"/>
       <c r="S19" s="73" t="n"/>
-      <c r="T19" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T19" s="73" t="inlineStr"/>
       <c r="U19" s="74" t="n"/>
       <c r="V19" s="75" t="n"/>
       <c r="W19" s="73" t="inlineStr">
@@ -3340,7 +3312,7 @@
       </c>
       <c r="K20" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzabile tramite selezione da un set di valori ammessi</t>
+          <t>Campo valorizzabile tramite selezione da un set di valori ammessi</t>
         </is>
       </c>
       <c r="L20" s="73" t="n"/>
@@ -3351,11 +3323,7 @@
       <c r="Q20" s="73" t="n"/>
       <c r="R20" s="73" t="n"/>
       <c r="S20" s="73" t="n"/>
-      <c r="T20" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T20" s="73" t="inlineStr"/>
       <c r="U20" s="74" t="n"/>
       <c r="V20" s="75" t="n"/>
       <c r="W20" s="73" t="inlineStr">
@@ -3400,7 +3368,7 @@
       </c>
       <c r="K21" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzato in automatico tramite dati recuperati da servizi esterni</t>
+          <t>Campo valorizzato in automatico tramite dati recuperati da servizi esterni</t>
         </is>
       </c>
       <c r="L21" s="73" t="n"/>
@@ -3411,11 +3379,7 @@
       <c r="Q21" s="73" t="n"/>
       <c r="R21" s="73" t="n"/>
       <c r="S21" s="73" t="n"/>
-      <c r="T21" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T21" s="73" t="inlineStr"/>
       <c r="U21" s="74" t="n"/>
       <c r="V21" s="75" t="n"/>
       <c r="W21" s="73" t="inlineStr">
@@ -3460,7 +3424,7 @@
       </c>
       <c r="K22" s="73" t="inlineStr">
         <is>
-          <t>l'applicativo effettua controlli preventivi sul dato inserito</t>
+          <t>L'applicativo effettua controlli preventivi sul dato inserito</t>
         </is>
       </c>
       <c r="L22" s="73" t="n"/>
@@ -3471,11 +3435,7 @@
       <c r="Q22" s="73" t="n"/>
       <c r="R22" s="73" t="n"/>
       <c r="S22" s="73" t="n"/>
-      <c r="T22" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T22" s="73" t="inlineStr"/>
       <c r="U22" s="74" t="n"/>
       <c r="V22" s="75" t="n"/>
       <c r="W22" s="73" t="inlineStr">
@@ -3520,7 +3480,7 @@
       </c>
       <c r="K23" s="73" t="inlineStr">
         <is>
-          <t>campo obbligatorio</t>
+          <t>Campo obbligatorio</t>
         </is>
       </c>
       <c r="L23" s="73" t="n"/>
@@ -3531,11 +3491,7 @@
       <c r="Q23" s="73" t="n"/>
       <c r="R23" s="73" t="n"/>
       <c r="S23" s="73" t="n"/>
-      <c r="T23" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T23" s="73" t="inlineStr"/>
       <c r="U23" s="74" t="n"/>
       <c r="V23" s="75" t="n"/>
       <c r="W23" s="73" t="inlineStr">
@@ -3580,7 +3536,7 @@
       </c>
       <c r="K24" s="73" t="inlineStr">
         <is>
-          <t>campo obbligatorio</t>
+          <t>Campo obbligatorio</t>
         </is>
       </c>
       <c r="L24" s="73" t="n"/>
@@ -3591,11 +3547,7 @@
       <c r="Q24" s="73" t="n"/>
       <c r="R24" s="73" t="n"/>
       <c r="S24" s="73" t="n"/>
-      <c r="T24" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T24" s="73" t="inlineStr"/>
       <c r="U24" s="74" t="n"/>
       <c r="V24" s="75" t="n"/>
       <c r="W24" s="73" t="inlineStr">
@@ -3640,7 +3592,7 @@
       </c>
       <c r="K25" s="73" t="inlineStr">
         <is>
-          <t>l'applicativo effettua controlli preventivi sul dato inserito</t>
+          <t>L'applicativo effettua controlli preventivi sul dato inserito</t>
         </is>
       </c>
       <c r="L25" s="73" t="n"/>
@@ -3651,11 +3603,7 @@
       <c r="Q25" s="73" t="n"/>
       <c r="R25" s="73" t="n"/>
       <c r="S25" s="73" t="n"/>
-      <c r="T25" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T25" s="73" t="inlineStr"/>
       <c r="U25" s="74" t="n"/>
       <c r="V25" s="75" t="n"/>
       <c r="W25" s="73" t="inlineStr">
@@ -3700,7 +3648,7 @@
       </c>
       <c r="K26" s="73" t="inlineStr">
         <is>
-          <t>campo obbligatorio</t>
+          <t>Campo obbligatorio</t>
         </is>
       </c>
       <c r="L26" s="73" t="n"/>
@@ -3711,11 +3659,7 @@
       <c r="Q26" s="73" t="n"/>
       <c r="R26" s="73" t="n"/>
       <c r="S26" s="73" t="n"/>
-      <c r="T26" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T26" s="73" t="inlineStr"/>
       <c r="U26" s="74" t="n"/>
       <c r="V26" s="75" t="n"/>
       <c r="W26" s="73" t="inlineStr">
@@ -3760,7 +3704,7 @@
       </c>
       <c r="K27" s="73" t="inlineStr">
         <is>
-          <t>campo obbligatorio</t>
+          <t>Campo obbligatorio</t>
         </is>
       </c>
       <c r="L27" s="73" t="n"/>
@@ -3771,11 +3715,7 @@
       <c r="Q27" s="73" t="n"/>
       <c r="R27" s="73" t="n"/>
       <c r="S27" s="73" t="n"/>
-      <c r="T27" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T27" s="73" t="inlineStr"/>
       <c r="U27" s="74" t="n"/>
       <c r="V27" s="75" t="n"/>
       <c r="W27" s="73" t="inlineStr">
@@ -3820,7 +3760,7 @@
       </c>
       <c r="K28" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzabile tramite selezione da un set di valori ammessi</t>
+          <t>Campo valorizzabile tramite selezione da un set di valori ammessi</t>
         </is>
       </c>
       <c r="L28" s="73" t="n"/>
@@ -3831,11 +3771,7 @@
       <c r="Q28" s="73" t="n"/>
       <c r="R28" s="73" t="n"/>
       <c r="S28" s="73" t="n"/>
-      <c r="T28" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T28" s="73" t="inlineStr"/>
       <c r="U28" s="74" t="n"/>
       <c r="V28" s="75" t="n"/>
       <c r="W28" s="73" t="inlineStr">
@@ -3880,7 +3816,7 @@
       </c>
       <c r="K29" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzato in automatico tramite dati recuperati da servizi esterni</t>
+          <t>Campo valorizzato in automatico tramite dati recuperati da servizi esterni</t>
         </is>
       </c>
       <c r="L29" s="73" t="n"/>
@@ -3891,11 +3827,7 @@
       <c r="Q29" s="73" t="n"/>
       <c r="R29" s="73" t="n"/>
       <c r="S29" s="73" t="n"/>
-      <c r="T29" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T29" s="73" t="inlineStr"/>
       <c r="U29" s="74" t="n"/>
       <c r="V29" s="75" t="n"/>
       <c r="W29" s="73" t="inlineStr">
@@ -3940,7 +3872,7 @@
       </c>
       <c r="K30" s="73" t="inlineStr">
         <is>
-          <t>l'applicativo effettua controlli preventivi sul dato inserito</t>
+          <t>L'applicativo effettua controlli preventivi sul dato inserito</t>
         </is>
       </c>
       <c r="L30" s="73" t="n"/>
@@ -3951,11 +3883,7 @@
       <c r="Q30" s="73" t="n"/>
       <c r="R30" s="73" t="n"/>
       <c r="S30" s="73" t="n"/>
-      <c r="T30" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T30" s="73" t="inlineStr"/>
       <c r="U30" s="74" t="n"/>
       <c r="V30" s="75" t="n"/>
       <c r="W30" s="73" t="inlineStr">
@@ -4000,7 +3928,7 @@
       </c>
       <c r="K31" s="73" t="inlineStr">
         <is>
-          <t>campo obbligatorio</t>
+          <t>Campo obbligatorio</t>
         </is>
       </c>
       <c r="L31" s="73" t="n"/>
@@ -4011,11 +3939,7 @@
       <c r="Q31" s="73" t="n"/>
       <c r="R31" s="73" t="n"/>
       <c r="S31" s="73" t="n"/>
-      <c r="T31" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T31" s="73" t="inlineStr"/>
       <c r="U31" s="74" t="n"/>
       <c r="V31" s="75" t="n"/>
       <c r="W31" s="73" t="inlineStr">
@@ -4060,7 +3984,7 @@
       </c>
       <c r="K32" s="73" t="inlineStr">
         <is>
-          <t>campo obbligatorio</t>
+          <t>Campo obbligatorio</t>
         </is>
       </c>
       <c r="L32" s="73" t="n"/>
@@ -4071,11 +3995,7 @@
       <c r="Q32" s="73" t="n"/>
       <c r="R32" s="73" t="n"/>
       <c r="S32" s="73" t="n"/>
-      <c r="T32" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T32" s="73" t="inlineStr"/>
       <c r="U32" s="74" t="n"/>
       <c r="V32" s="75" t="n"/>
       <c r="W32" s="73" t="inlineStr">
@@ -4120,7 +4040,7 @@
       </c>
       <c r="K33" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzato in automatico tramite dati recuperati da servizi esterni</t>
+          <t>Campo valorizzato in automatico tramite dati recuperati da servizi esterni</t>
         </is>
       </c>
       <c r="L33" s="73" t="n"/>
@@ -4131,11 +4051,7 @@
       <c r="Q33" s="73" t="n"/>
       <c r="R33" s="73" t="n"/>
       <c r="S33" s="73" t="n"/>
-      <c r="T33" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T33" s="73" t="inlineStr"/>
       <c r="U33" s="74" t="n"/>
       <c r="V33" s="75" t="n"/>
       <c r="W33" s="73" t="inlineStr">
@@ -4180,7 +4096,7 @@
       </c>
       <c r="K34" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzato di default</t>
+          <t>Campo valorizzato di default</t>
         </is>
       </c>
       <c r="L34" s="73" t="n"/>
@@ -4191,11 +4107,7 @@
       <c r="Q34" s="73" t="n"/>
       <c r="R34" s="73" t="n"/>
       <c r="S34" s="73" t="n"/>
-      <c r="T34" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T34" s="73" t="inlineStr"/>
       <c r="U34" s="74" t="n"/>
       <c r="V34" s="75" t="n"/>
       <c r="W34" s="73" t="inlineStr">
@@ -4240,7 +4152,7 @@
       </c>
       <c r="K35" s="73" t="inlineStr">
         <is>
-          <t>campo obbligatorio</t>
+          <t>Campo obbligatorio</t>
         </is>
       </c>
       <c r="L35" s="73" t="n"/>
@@ -4251,11 +4163,7 @@
       <c r="Q35" s="73" t="n"/>
       <c r="R35" s="73" t="n"/>
       <c r="S35" s="73" t="n"/>
-      <c r="T35" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T35" s="73" t="inlineStr"/>
       <c r="U35" s="74" t="n"/>
       <c r="V35" s="75" t="n"/>
       <c r="W35" s="73" t="inlineStr">
@@ -4300,7 +4208,7 @@
       </c>
       <c r="K36" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzato di default</t>
+          <t>Campo valorizzato di default</t>
         </is>
       </c>
       <c r="L36" s="73" t="n"/>
@@ -4311,11 +4219,7 @@
       <c r="Q36" s="73" t="n"/>
       <c r="R36" s="73" t="n"/>
       <c r="S36" s="73" t="n"/>
-      <c r="T36" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T36" s="73" t="inlineStr"/>
       <c r="U36" s="74" t="n"/>
       <c r="V36" s="75" t="n"/>
       <c r="W36" s="73" t="inlineStr">
@@ -4360,7 +4264,7 @@
       </c>
       <c r="K37" s="73" t="inlineStr">
         <is>
-          <t>campo obbligatorio</t>
+          <t>Campo obbligatorio</t>
         </is>
       </c>
       <c r="L37" s="73" t="n"/>
@@ -4371,11 +4275,7 @@
       <c r="Q37" s="73" t="n"/>
       <c r="R37" s="73" t="n"/>
       <c r="S37" s="73" t="n"/>
-      <c r="T37" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T37" s="73" t="inlineStr"/>
       <c r="U37" s="74" t="n"/>
       <c r="V37" s="75" t="n"/>
       <c r="W37" s="73" t="inlineStr">
@@ -4420,7 +4320,7 @@
       </c>
       <c r="K38" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzabile tramite selezione da un set di valori ammessi</t>
+          <t>Campo valorizzabile tramite selezione da un set di valori ammessi</t>
         </is>
       </c>
       <c r="L38" s="73" t="n"/>
@@ -4431,11 +4331,7 @@
       <c r="Q38" s="73" t="n"/>
       <c r="R38" s="73" t="n"/>
       <c r="S38" s="73" t="n"/>
-      <c r="T38" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T38" s="73" t="inlineStr"/>
       <c r="U38" s="74" t="n"/>
       <c r="V38" s="75" t="n"/>
       <c r="W38" s="73" t="inlineStr">
@@ -4480,7 +4376,7 @@
       </c>
       <c r="K39" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzato di default</t>
+          <t>Campo valorizzato di default</t>
         </is>
       </c>
       <c r="L39" s="73" t="n"/>
@@ -4491,11 +4387,7 @@
       <c r="Q39" s="73" t="n"/>
       <c r="R39" s="73" t="n"/>
       <c r="S39" s="73" t="n"/>
-      <c r="T39" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T39" s="73" t="inlineStr"/>
       <c r="U39" s="74" t="n"/>
       <c r="V39" s="75" t="n"/>
       <c r="W39" s="73" t="inlineStr">
@@ -4506,7 +4398,7 @@
     </row>
     <row r="40" ht="11" customHeight="1" s="46" thickBot="1">
       <c r="A40" s="35" t="n">
-        <v>448</v>
+        <v>191</v>
       </c>
       <c r="B40" s="35" t="inlineStr">
         <is>
@@ -4515,38 +4407,39 @@
       </c>
       <c r="C40" s="41" t="inlineStr">
         <is>
-          <t>RSA</t>
+          <t>LAB</t>
         </is>
       </c>
       <c r="D40" s="35" t="inlineStr">
         <is>
-          <t>VALIDAZIONE_CDA2_RSA_CT24</t>
+          <t>VALIDAZIONE_CDA2_LAB_TRASF_CT1</t>
         </is>
       </c>
       <c r="E40" s="43" t="inlineStr">
         <is>
-          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+          <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Laboratorio dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST- OK" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
         </is>
       </c>
       <c r="F40" s="67" t="inlineStr">
         <is>
-          <t>2025-11-10</t>
+          <t>2025-11-12</t>
         </is>
       </c>
       <c r="G40" s="67" t="inlineStr">
         <is>
-          <t>2025-11-10T12:05:11Z</t>
+          <t>2025-11-12T12:59:34Z</t>
         </is>
       </c>
       <c r="H40" s="67" t="inlineStr">
         <is>
-          <t>18c021c20606c2e0e5e99bc61fe4464e</t>
+          <t>aa7c3602c0291a701254b79bbd26f5f4</t>
         </is>
       </c>
       <c r="I40" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.af3ba333d6e1f53aa0c6857d748bda8c628b4e1b15ab0568357c9ae9639dd0e9.c5548faeb7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.f7f4ab3b8d8704ba25d31a70c62517fff99f77bbc4090947c507ca4a691dd0d9.4a3fab18ec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J40" s="68" t="inlineStr">
@@ -4578,7 +4471,7 @@
     </row>
     <row r="41" ht="11" customHeight="1" s="46" thickBot="1">
       <c r="A41" s="35" t="n">
-        <v>449</v>
+        <v>376</v>
       </c>
       <c r="B41" s="35" t="inlineStr">
         <is>
@@ -4587,38 +4480,39 @@
       </c>
       <c r="C41" s="41" t="inlineStr">
         <is>
-          <t>RSA</t>
+          <t>LAB</t>
         </is>
       </c>
       <c r="D41" s="35" t="inlineStr">
         <is>
-          <t>VALIDAZIONE_CDA2_RSA_CT25</t>
+          <t>VALIDAZIONE_CDA2_LAB_TRASF_CT2</t>
         </is>
       </c>
       <c r="E41" s="43" t="inlineStr">
         <is>
-          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+          <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Laboratorio dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST OK - HLA" riportata nei documenti "Caso di test - Trasfusionale" e "CDA2_Trasfusionale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
         </is>
       </c>
       <c r="F41" s="67" t="inlineStr">
         <is>
-          <t>2025-11-10</t>
+          <t>2025-11-12</t>
         </is>
       </c>
       <c r="G41" s="67" t="inlineStr">
         <is>
-          <t>2025-11-10T12:05:15Z</t>
+          <t>2025-11-12T12:59:34Z</t>
         </is>
       </c>
       <c r="H41" s="67" t="inlineStr">
         <is>
-          <t>f55de0f0e712cccb42efc6d0d12ce3e5</t>
+          <t>bd11c5032817ab825f8752aa64e10550</t>
         </is>
       </c>
       <c r="I41" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.016921dc02d53cb2079085d39046bd2c3869682dd78adbcaedcec4ecd8e5e462.1db14c9b19^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.b94fd81cb684439fda3ee259a70d9eee980028dbf2ec2a7377d67a65dc3431a3.159dcd0e2a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J41" s="68" t="inlineStr">
@@ -4650,7 +4544,7 @@
     </row>
     <row r="42" ht="11" customHeight="1" s="46" thickBot="1">
       <c r="A42" s="35" t="n">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B42" s="35" t="inlineStr">
         <is>
@@ -4659,39 +4553,38 @@
       </c>
       <c r="C42" s="41" t="inlineStr">
         <is>
-          <t>LAB</t>
+          <t>RSA</t>
         </is>
       </c>
       <c r="D42" s="35" t="inlineStr">
         <is>
-          <t>VALIDAZIONE_CDA2_LAB_CT17</t>
+          <t>VALIDAZIONE_CDA2_RSA_CT24</t>
         </is>
       </c>
       <c r="E42" s="43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-Il Documento CDA2 Laboratorio dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 17" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
-</t>
+          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
         </is>
       </c>
       <c r="F42" s="67" t="inlineStr">
         <is>
-          <t>2025-11-10</t>
+          <t>2025-11-12</t>
         </is>
       </c>
       <c r="G42" s="67" t="inlineStr">
         <is>
-          <t>2025-11-10T12:04:12Z</t>
+          <t>2025-11-12T13:00:27Z</t>
         </is>
       </c>
       <c r="H42" s="67" t="inlineStr">
         <is>
-          <t>63be817b6e6003022e9531f8887cd107</t>
+          <t>0dd2a0732bb4a0b23840e957d8e9b6db</t>
         </is>
       </c>
       <c r="I42" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.fbc9fcc7606df615b8cd4d9f200ab7696308486b44c965e9f171af26f58bf47b.fee419fcd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.0f3bdeaf7eec4d92e8fafcd8a7491c473d2c8ba772ac65b75631363ae69bdbdc.7db9590748^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J42" s="68" t="inlineStr">
@@ -4723,147 +4616,172 @@
     </row>
     <row r="43" ht="11" customHeight="1" s="46" thickBot="1">
       <c r="A43" s="35" t="n">
+        <v>449</v>
+      </c>
+      <c r="B43" s="35" t="inlineStr">
+        <is>
+          <t>VALIDAZIONE</t>
+        </is>
+      </c>
+      <c r="C43" s="41" t="inlineStr">
+        <is>
+          <t>RSA</t>
+        </is>
+      </c>
+      <c r="D43" s="35" t="inlineStr">
+        <is>
+          <t>VALIDAZIONE_CDA2_RSA_CT25</t>
+        </is>
+      </c>
+      <c r="E43" s="43" t="inlineStr">
+        <is>
+          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 25" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+        </is>
+      </c>
+      <c r="F43" s="67" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+      <c r="G43" s="67" t="inlineStr">
+        <is>
+          <t>2025-11-12T13:00:30Z</t>
+        </is>
+      </c>
+      <c r="H43" s="67" t="inlineStr">
+        <is>
+          <t>16a68ee156c2a32425c33f2881148301</t>
+        </is>
+      </c>
+      <c r="I43" s="81" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.fb6e1fd98bacccb78021a5e9714d4a784d681cc094fc4070bd1c45e61dbda171.b5ccbeca07^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+        </is>
+      </c>
+      <c r="J43" s="68" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="K43" s="68" t="n"/>
+      <c r="L43" s="68" t="n"/>
+      <c r="M43" s="68" t="n"/>
+      <c r="N43" s="68" t="n"/>
+      <c r="O43" s="68" t="n"/>
+      <c r="P43" s="68" t="n"/>
+      <c r="Q43" s="68" t="n"/>
+      <c r="R43" s="68" t="n"/>
+      <c r="S43" s="68" t="n"/>
+      <c r="T43" s="68" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="U43" s="69" t="n"/>
+      <c r="V43" s="70" t="n"/>
+      <c r="W43" s="68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="11" customHeight="1" s="46" thickBot="1">
+      <c r="A44" s="35" t="n">
+        <v>452</v>
+      </c>
+      <c r="B44" s="35" t="inlineStr">
+        <is>
+          <t>VALIDAZIONE</t>
+        </is>
+      </c>
+      <c r="C44" s="41" t="inlineStr">
+        <is>
+          <t>LAB</t>
+        </is>
+      </c>
+      <c r="D44" s="35" t="inlineStr">
+        <is>
+          <t>VALIDAZIONE_CDA2_LAB_CT17</t>
+        </is>
+      </c>
+      <c r="E44" s="43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+Il Documento CDA2 Laboratorio dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 17" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
+</t>
+        </is>
+      </c>
+      <c r="F44" s="67" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+      <c r="G44" s="67" t="inlineStr">
+        <is>
+          <t>2025-11-12T12:59:30Z</t>
+        </is>
+      </c>
+      <c r="H44" s="67" t="inlineStr">
+        <is>
+          <t>ad5a45c05e21a0a4ded5da2fde1b2f96</t>
+        </is>
+      </c>
+      <c r="I44" s="81" t="inlineStr">
+        <is>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.6e198c9883a9b3ef55308cf73b84439406545ff76daba9afe2847bba9375dd0f.ad4d1132c3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+        </is>
+      </c>
+      <c r="J44" s="68" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="K44" s="68" t="n"/>
+      <c r="L44" s="68" t="n"/>
+      <c r="M44" s="68" t="n"/>
+      <c r="N44" s="68" t="n"/>
+      <c r="O44" s="68" t="n"/>
+      <c r="P44" s="68" t="n"/>
+      <c r="Q44" s="68" t="n"/>
+      <c r="R44" s="68" t="n"/>
+      <c r="S44" s="68" t="n"/>
+      <c r="T44" s="68" t="inlineStr">
+        <is>
+          <t>PASS</t>
+        </is>
+      </c>
+      <c r="U44" s="69" t="n"/>
+      <c r="V44" s="70" t="n"/>
+      <c r="W44" s="68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="11" customHeight="1" s="46" thickBot="1">
+      <c r="A45" s="35" t="n">
         <v>461</v>
       </c>
-      <c r="B43" s="35" t="inlineStr">
+      <c r="B45" s="35" t="inlineStr">
         <is>
           <t>VALIDAZIONE</t>
         </is>
       </c>
-      <c r="C43" s="41" t="inlineStr">
+      <c r="C45" s="41" t="inlineStr">
         <is>
           <t>RSA</t>
         </is>
       </c>
-      <c r="D43" s="35" t="inlineStr">
+      <c r="D45" s="35" t="inlineStr">
         <is>
           <t>VALIDAZIONE_CDA2_RSA_CT26_KO</t>
         </is>
       </c>
-      <c r="E43" s="43" t="inlineStr">
+      <c r="E45" s="43" t="inlineStr">
         <is>
           <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 26" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-        </is>
-      </c>
-      <c r="F43" s="82" t="n"/>
-      <c r="G43" s="82" t="n"/>
-      <c r="H43" s="82" t="n"/>
-      <c r="I43" s="82" t="n"/>
-      <c r="J43" s="73" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K43" s="73" t="inlineStr">
-        <is>
-          <t>campo valorizzabile tramite selezione da un set di valori ammessi</t>
-        </is>
-      </c>
-      <c r="L43" s="82" t="n"/>
-      <c r="M43" s="73" t="n"/>
-      <c r="N43" s="73" t="n"/>
-      <c r="O43" s="82" t="n"/>
-      <c r="P43" s="73" t="n"/>
-      <c r="Q43" s="73" t="n"/>
-      <c r="R43" s="73" t="n"/>
-      <c r="S43" s="82" t="n"/>
-      <c r="T43" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="U43" s="82" t="n"/>
-      <c r="V43" s="82" t="n"/>
-      <c r="W43" s="82" t="inlineStr">
-        <is>
-          <t>KO</t>
-        </is>
-      </c>
-    </row>
-    <row r="44" ht="11" customHeight="1" s="46" thickBot="1">
-      <c r="A44" s="35" t="n">
-        <v>466</v>
-      </c>
-      <c r="B44" s="35" t="inlineStr">
-        <is>
-          <t>VALIDAZIONE</t>
-        </is>
-      </c>
-      <c r="C44" s="41" t="inlineStr">
-        <is>
-          <t>LAB</t>
-        </is>
-      </c>
-      <c r="D44" s="35" t="inlineStr">
-        <is>
-          <t>VALIDAZIONE_CDA2_LAB_CT18</t>
-        </is>
-      </c>
-      <c r="E44" s="44" t="inlineStr">
-        <is>
-          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO.xlsx" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-        </is>
-      </c>
-      <c r="F44" s="82" t="n"/>
-      <c r="G44" s="82" t="n"/>
-      <c r="H44" s="82" t="n"/>
-      <c r="I44" s="82" t="n"/>
-      <c r="J44" s="73" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="K44" s="73" t="inlineStr">
-        <is>
-          <t>l'applicativo effettua controlli preventivi sul dato inserito</t>
-        </is>
-      </c>
-      <c r="L44" s="82" t="n"/>
-      <c r="M44" s="73" t="n"/>
-      <c r="N44" s="73" t="n"/>
-      <c r="O44" s="82" t="n"/>
-      <c r="P44" s="73" t="n"/>
-      <c r="Q44" s="73" t="n"/>
-      <c r="R44" s="73" t="n"/>
-      <c r="S44" s="82" t="n"/>
-      <c r="T44" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="U44" s="82" t="n"/>
-      <c r="V44" s="82" t="n"/>
-      <c r="W44" s="82" t="inlineStr">
-        <is>
-          <t>KO</t>
-        </is>
-      </c>
-    </row>
-    <row r="45" ht="11" customHeight="1" s="46" thickBot="1">
-      <c r="A45" s="35" t="n">
-        <v>468</v>
-      </c>
-      <c r="B45" s="35" t="inlineStr">
-        <is>
-          <t>VALIDAZIONE</t>
-        </is>
-      </c>
-      <c r="C45" s="41" t="inlineStr">
-        <is>
-          <t>RSA</t>
-        </is>
-      </c>
-      <c r="D45" s="35" t="inlineStr">
-        <is>
-          <t>VALIDAZIONE_CDA2_RSA_CT27_KO</t>
-        </is>
-      </c>
-      <c r="E45" s="43" t="inlineStr">
-        <is>
-          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 27" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
         </is>
       </c>
       <c r="F45" s="82" t="n"/>
@@ -4877,7 +4795,7 @@
       </c>
       <c r="K45" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzato di default</t>
+          <t>Campo valorizzabile tramite selezione da un set di valori ammessi</t>
         </is>
       </c>
       <c r="L45" s="82" t="n"/>
@@ -4888,11 +4806,7 @@
       <c r="Q45" s="73" t="n"/>
       <c r="R45" s="73" t="n"/>
       <c r="S45" s="82" t="n"/>
-      <c r="T45" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="T45" s="73" t="inlineStr"/>
       <c r="U45" s="82" t="n"/>
       <c r="V45" s="82" t="n"/>
       <c r="W45" s="82" t="inlineStr">
@@ -4903,7 +4817,7 @@
     </row>
     <row r="46" ht="11" customHeight="1" s="46" thickBot="1">
       <c r="A46" s="35" t="n">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="B46" s="35" t="inlineStr">
         <is>
@@ -4915,21 +4829,21 @@
           <t>LAB</t>
         </is>
       </c>
-      <c r="D46" s="41" t="inlineStr">
-        <is>
-          <t>VALIDAZIONE_CDA2_LAB_CT19_KO</t>
-        </is>
-      </c>
-      <c r="E46" s="43" t="inlineStr">
-        <is>
-          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-        </is>
-      </c>
-      <c r="F46" s="71" t="n"/>
-      <c r="G46" s="71" t="n"/>
-      <c r="H46" s="71" t="n"/>
-      <c r="I46" s="72" t="n"/>
+      <c r="D46" s="35" t="inlineStr">
+        <is>
+          <t>VALIDAZIONE_CDA2_LAB_CT18</t>
+        </is>
+      </c>
+      <c r="E46" s="44" t="inlineStr">
+        <is>
+          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 18" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO.xlsx" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+        </is>
+      </c>
+      <c r="F46" s="82" t="n"/>
+      <c r="G46" s="82" t="n"/>
+      <c r="H46" s="82" t="n"/>
+      <c r="I46" s="82" t="n"/>
       <c r="J46" s="73" t="inlineStr">
         <is>
           <t>NO</t>
@@ -4937,25 +4851,21 @@
       </c>
       <c r="K46" s="73" t="inlineStr">
         <is>
-          <t>l'applicativo effettua controlli preventivi sul dato inserito</t>
-        </is>
-      </c>
-      <c r="L46" s="73" t="n"/>
+          <t>L'applicativo effettua controlli preventivi sul dato inserito</t>
+        </is>
+      </c>
+      <c r="L46" s="82" t="n"/>
       <c r="M46" s="73" t="n"/>
       <c r="N46" s="73" t="n"/>
-      <c r="O46" s="73" t="n"/>
+      <c r="O46" s="82" t="n"/>
       <c r="P46" s="73" t="n"/>
       <c r="Q46" s="73" t="n"/>
       <c r="R46" s="73" t="n"/>
-      <c r="S46" s="73" t="n"/>
-      <c r="T46" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="U46" s="74" t="n"/>
-      <c r="V46" s="75" t="n"/>
-      <c r="W46" s="73" t="inlineStr">
+      <c r="S46" s="82" t="n"/>
+      <c r="T46" s="73" t="inlineStr"/>
+      <c r="U46" s="82" t="n"/>
+      <c r="V46" s="82" t="n"/>
+      <c r="W46" s="82" t="inlineStr">
         <is>
           <t>KO</t>
         </is>
@@ -4963,7 +4873,7 @@
     </row>
     <row r="47" ht="11" customHeight="1" s="46" thickBot="1">
       <c r="A47" s="35" t="n">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="B47" s="35" t="inlineStr">
         <is>
@@ -4977,19 +4887,19 @@
       </c>
       <c r="D47" s="35" t="inlineStr">
         <is>
-          <t>VALIDAZIONE_CDA2_RSA_CT28_KO</t>
+          <t>VALIDAZIONE_CDA2_RSA_CT27_KO</t>
         </is>
       </c>
       <c r="E47" s="43" t="inlineStr">
         <is>
-          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
-I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 28" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-        </is>
-      </c>
-      <c r="F47" s="71" t="n"/>
-      <c r="G47" s="71" t="n"/>
-      <c r="H47" s="71" t="n"/>
-      <c r="I47" s="72" t="n"/>
+          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 27" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+        </is>
+      </c>
+      <c r="F47" s="82" t="n"/>
+      <c r="G47" s="82" t="n"/>
+      <c r="H47" s="82" t="n"/>
+      <c r="I47" s="82" t="n"/>
       <c r="J47" s="73" t="inlineStr">
         <is>
           <t>NO</t>
@@ -4997,69 +4907,137 @@
       </c>
       <c r="K47" s="73" t="inlineStr">
         <is>
-          <t>campo valorizzabile tramite selezione da un set di valori ammessi</t>
-        </is>
-      </c>
-      <c r="L47" s="73" t="n"/>
+          <t>Campo valorizzato di default</t>
+        </is>
+      </c>
+      <c r="L47" s="82" t="n"/>
       <c r="M47" s="73" t="n"/>
       <c r="N47" s="73" t="n"/>
-      <c r="O47" s="73" t="n"/>
+      <c r="O47" s="82" t="n"/>
       <c r="P47" s="73" t="n"/>
       <c r="Q47" s="73" t="n"/>
       <c r="R47" s="73" t="n"/>
-      <c r="S47" s="73" t="n"/>
-      <c r="T47" s="73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="U47" s="74" t="n"/>
-      <c r="V47" s="75" t="n"/>
-      <c r="W47" s="73" t="inlineStr">
+      <c r="S47" s="82" t="n"/>
+      <c r="T47" s="73" t="inlineStr"/>
+      <c r="U47" s="82" t="n"/>
+      <c r="V47" s="82" t="n"/>
+      <c r="W47" s="82" t="inlineStr">
         <is>
           <t>KO</t>
         </is>
       </c>
     </row>
     <row r="48" ht="11" customHeight="1" s="46" thickBot="1">
-      <c r="F48" s="6" t="n"/>
-      <c r="G48" s="6" t="n"/>
-      <c r="H48" s="6" t="n"/>
-      <c r="I48" s="6" t="n"/>
-      <c r="J48" s="7" t="n"/>
-      <c r="K48" s="7" t="n"/>
-      <c r="L48" s="7" t="n"/>
-      <c r="M48" s="7" t="n"/>
-      <c r="N48" s="7" t="n"/>
-      <c r="O48" s="7" t="n"/>
-      <c r="P48" s="7" t="n"/>
-      <c r="Q48" s="7" t="n"/>
-      <c r="R48" s="7" t="n"/>
-      <c r="S48" s="7" t="n"/>
-      <c r="T48" s="7" t="n"/>
-      <c r="U48" s="8" t="n"/>
-      <c r="V48" s="2" t="n"/>
-      <c r="W48" s="9" t="n"/>
+      <c r="A48" s="35" t="n">
+        <v>473</v>
+      </c>
+      <c r="B48" s="35" t="inlineStr">
+        <is>
+          <t>VALIDAZIONE</t>
+        </is>
+      </c>
+      <c r="C48" s="41" t="inlineStr">
+        <is>
+          <t>LAB</t>
+        </is>
+      </c>
+      <c r="D48" s="41" t="inlineStr">
+        <is>
+          <t>VALIDAZIONE_CDA2_LAB_CT19_KO</t>
+        </is>
+      </c>
+      <c r="E48" s="43" t="inlineStr">
+        <is>
+          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+        </is>
+      </c>
+      <c r="F48" s="71" t="n"/>
+      <c r="G48" s="71" t="n"/>
+      <c r="H48" s="71" t="n"/>
+      <c r="I48" s="72" t="n"/>
+      <c r="J48" s="73" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="K48" s="73" t="inlineStr">
+        <is>
+          <t>L'applicativo effettua controlli preventivi sul dato inserito</t>
+        </is>
+      </c>
+      <c r="L48" s="73" t="n"/>
+      <c r="M48" s="73" t="n"/>
+      <c r="N48" s="73" t="n"/>
+      <c r="O48" s="73" t="n"/>
+      <c r="P48" s="73" t="n"/>
+      <c r="Q48" s="73" t="n"/>
+      <c r="R48" s="73" t="n"/>
+      <c r="S48" s="73" t="n"/>
+      <c r="T48" s="73" t="inlineStr"/>
+      <c r="U48" s="74" t="n"/>
+      <c r="V48" s="75" t="n"/>
+      <c r="W48" s="73" t="inlineStr">
+        <is>
+          <t>KO</t>
+        </is>
+      </c>
     </row>
     <row r="49" ht="11" customHeight="1" s="46" thickBot="1">
-      <c r="F49" s="6" t="n"/>
-      <c r="G49" s="6" t="n"/>
-      <c r="H49" s="6" t="n"/>
-      <c r="I49" s="6" t="n"/>
-      <c r="J49" s="7" t="n"/>
-      <c r="K49" s="7" t="n"/>
-      <c r="L49" s="7" t="n"/>
-      <c r="M49" s="7" t="n"/>
-      <c r="N49" s="7" t="n"/>
-      <c r="O49" s="7" t="n"/>
-      <c r="P49" s="7" t="n"/>
-      <c r="Q49" s="7" t="n"/>
-      <c r="R49" s="7" t="n"/>
-      <c r="S49" s="7" t="n"/>
-      <c r="T49" s="7" t="n"/>
-      <c r="U49" s="8" t="n"/>
-      <c r="V49" s="2" t="n"/>
-      <c r="W49" s="9" t="n"/>
+      <c r="A49" s="35" t="n">
+        <v>475</v>
+      </c>
+      <c r="B49" s="35" t="inlineStr">
+        <is>
+          <t>VALIDAZIONE</t>
+        </is>
+      </c>
+      <c r="C49" s="41" t="inlineStr">
+        <is>
+          <t>RSA</t>
+        </is>
+      </c>
+      <c r="D49" s="35" t="inlineStr">
+        <is>
+          <t>VALIDAZIONE_CDA2_RSA_CT28_KO</t>
+        </is>
+      </c>
+      <c r="E49" s="43" t="inlineStr">
+        <is>
+          <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
+I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 28" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+        </is>
+      </c>
+      <c r="F49" s="71" t="n"/>
+      <c r="G49" s="71" t="n"/>
+      <c r="H49" s="71" t="n"/>
+      <c r="I49" s="72" t="n"/>
+      <c r="J49" s="73" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="K49" s="73" t="inlineStr">
+        <is>
+          <t>Campo valorizzabile tramite selezione da un set di valori ammessi</t>
+        </is>
+      </c>
+      <c r="L49" s="73" t="n"/>
+      <c r="M49" s="73" t="n"/>
+      <c r="N49" s="73" t="n"/>
+      <c r="O49" s="73" t="n"/>
+      <c r="P49" s="73" t="n"/>
+      <c r="Q49" s="73" t="n"/>
+      <c r="R49" s="73" t="n"/>
+      <c r="S49" s="73" t="n"/>
+      <c r="T49" s="73" t="inlineStr"/>
+      <c r="U49" s="74" t="n"/>
+      <c r="V49" s="75" t="n"/>
+      <c r="W49" s="73" t="inlineStr">
+        <is>
+          <t>KO</t>
+        </is>
+      </c>
     </row>
     <row r="50" ht="11" customHeight="1" s="46" thickBot="1">
       <c r="F50" s="6" t="n"/>
@@ -7782,10 +7760,44 @@
       <c r="W185" s="9" t="n"/>
     </row>
     <row r="186" ht="14.25" customHeight="1" s="46" thickBot="1">
-      <c r="W186" s="7" t="n"/>
+      <c r="F186" s="6" t="n"/>
+      <c r="G186" s="6" t="n"/>
+      <c r="H186" s="6" t="n"/>
+      <c r="I186" s="6" t="n"/>
+      <c r="J186" s="7" t="n"/>
+      <c r="K186" s="7" t="n"/>
+      <c r="L186" s="7" t="n"/>
+      <c r="M186" s="7" t="n"/>
+      <c r="N186" s="7" t="n"/>
+      <c r="O186" s="7" t="n"/>
+      <c r="P186" s="7" t="n"/>
+      <c r="Q186" s="7" t="n"/>
+      <c r="R186" s="7" t="n"/>
+      <c r="S186" s="7" t="n"/>
+      <c r="T186" s="7" t="n"/>
+      <c r="U186" s="8" t="n"/>
+      <c r="V186" s="2" t="n"/>
+      <c r="W186" s="9" t="n"/>
     </row>
     <row r="187" ht="14.25" customHeight="1" s="46" thickBot="1">
-      <c r="W187" s="7" t="n"/>
+      <c r="F187" s="6" t="n"/>
+      <c r="G187" s="6" t="n"/>
+      <c r="H187" s="6" t="n"/>
+      <c r="I187" s="6" t="n"/>
+      <c r="J187" s="7" t="n"/>
+      <c r="K187" s="7" t="n"/>
+      <c r="L187" s="7" t="n"/>
+      <c r="M187" s="7" t="n"/>
+      <c r="N187" s="7" t="n"/>
+      <c r="O187" s="7" t="n"/>
+      <c r="P187" s="7" t="n"/>
+      <c r="Q187" s="7" t="n"/>
+      <c r="R187" s="7" t="n"/>
+      <c r="S187" s="7" t="n"/>
+      <c r="T187" s="7" t="n"/>
+      <c r="U187" s="8" t="n"/>
+      <c r="V187" s="2" t="n"/>
+      <c r="W187" s="9" t="n"/>
     </row>
     <row r="188" ht="14.25" customHeight="1" s="46" thickBot="1">
       <c r="W188" s="7" t="n"/>
@@ -9032,8 +9044,12 @@
     <row r="602" ht="14.25" customHeight="1" s="46">
       <c r="W602" s="7" t="n"/>
     </row>
-    <row r="603" ht="14.25" customHeight="1" s="46"/>
-    <row r="604" ht="14.25" customHeight="1" s="46"/>
+    <row r="603" ht="14.25" customHeight="1" s="46">
+      <c r="W603" s="7" t="n"/>
+    </row>
+    <row r="604" ht="14.25" customHeight="1" s="46">
+      <c r="W604" s="7" t="n"/>
+    </row>
     <row r="605" ht="14.25" customHeight="1" s="46"/>
     <row r="606" ht="14.25" customHeight="1" s="46"/>
     <row r="607" ht="14.25" customHeight="1" s="46"/>

</xml_diff>

<commit_message>
Fix test [452, 376, 4, 448, 191, 449]
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.56/report-checklist.xlsx
+++ b/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.56/report-checklist.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="33720" yWindow="975" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Istruzioni Compilazione" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Prerequisiti" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestCases" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LISTA VALORI" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="Istruzioni Compilazione" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Prerequisiti" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TestCases" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="LISTA VALORI" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Summary" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'TestCases'!$A$9:$W$192</definedName>
@@ -2627,22 +2627,22 @@
       </c>
       <c r="F10" s="66" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="G10" s="66" t="inlineStr">
         <is>
-          <t>2025-11-17T10:24:03Z</t>
+          <t>2025-11-20T09:36:13Z</t>
         </is>
       </c>
       <c r="H10" s="66" t="inlineStr">
         <is>
-          <t>a4fc5f3a4c483a2095d7fcaa46d7c54a</t>
+          <t>aa1e24be850220621e4bd400733d8957</t>
         </is>
       </c>
       <c r="I10" s="67" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.b63214f7c224a0da7d39e69c3ad7634c3b08132e2c53e6a77312b0718274f857.73a81ed972^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.206da0e5a5a596b3faa12030c1aef93330a218ee42be85a8a12e9f3ede6cf877.04aa7a6a73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J10" s="68" t="inlineStr">
@@ -2935,12 +2935,12 @@
       </c>
       <c r="F15" s="76" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="G15" s="76" t="inlineStr">
         <is>
-          <t>2025-11-17T10:25:10Z</t>
+          <t>2025-11-20T09:37:19Z</t>
         </is>
       </c>
       <c r="H15" s="76" t="inlineStr">
@@ -3035,12 +3035,12 @@
       </c>
       <c r="F16" s="76" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="G16" s="76" t="inlineStr">
         <is>
-          <t>2025-11-17T10:25:10Z</t>
+          <t>2025-11-20T09:37:19Z</t>
         </is>
       </c>
       <c r="H16" s="76" t="inlineStr">
@@ -4424,22 +4424,22 @@
       </c>
       <c r="F40" s="67" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="G40" s="67" t="inlineStr">
         <is>
-          <t>2025-11-17T10:24:10Z</t>
+          <t>2025-11-20T09:36:20Z</t>
         </is>
       </c>
       <c r="H40" s="67" t="inlineStr">
         <is>
-          <t>cf907f803277a6f7504252205cb83f68</t>
+          <t>8564ac9347687d4a355e2dd0552e7004</t>
         </is>
       </c>
       <c r="I40" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.b171cbd02273cd40a492a98a9d0c9d518bf752c7f4a77119df4fae3e27255216.7ba6178d48^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.30406e6567059ad7e9e67de27e479b6fd3a38429dfe83af0291c3c6d34d86e0c.2d94ef14fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J40" s="68" t="inlineStr">
@@ -4497,22 +4497,22 @@
       </c>
       <c r="F41" s="67" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="G41" s="67" t="inlineStr">
         <is>
-          <t>2025-11-17T10:24:11Z</t>
+          <t>2025-11-20T09:36:20Z</t>
         </is>
       </c>
       <c r="H41" s="67" t="inlineStr">
         <is>
-          <t>410382fdc8a003355832b71d4341077d</t>
+          <t>192a9b156d7d54ec4cac6f58595967f6</t>
         </is>
       </c>
       <c r="I41" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.296865d9c6120a0aa0a254819d76164496c43c3dc013c00548e6c5b46f86d56e.774f7506d9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.208a06f1bb78b35c2631ad3d6bb87d030df622ece4aedc74ceabd822bf77e4a9.dee1dd0079^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J41" s="68" t="inlineStr">
@@ -4569,22 +4569,22 @@
       </c>
       <c r="F42" s="67" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="G42" s="67" t="inlineStr">
         <is>
-          <t>2025-11-17T10:25:03Z</t>
+          <t>2025-11-20T09:37:11Z</t>
         </is>
       </c>
       <c r="H42" s="67" t="inlineStr">
         <is>
-          <t>2f8daab1b7d1062385a41e9cd0fa777a</t>
+          <t>9f8f2e4228bb8ed3a74164590e7b601f</t>
         </is>
       </c>
       <c r="I42" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.96dbc96f2ceb24dea37ee1d9ee51f034f8598e4b5ea7063b2680cd853462dc67.922d93bbab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.c2135097a224aaaa6a9c09a5d4643ff57410e7a2761a60f422f5ad040f1b440b.37ff88e20b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J42" s="68" t="inlineStr">
@@ -4641,22 +4641,22 @@
       </c>
       <c r="F43" s="67" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="G43" s="67" t="inlineStr">
         <is>
-          <t>2025-11-17T10:25:06Z</t>
+          <t>2025-11-20T09:37:15Z</t>
         </is>
       </c>
       <c r="H43" s="67" t="inlineStr">
         <is>
-          <t>76fdeb8c3e234d6d6044f07dbcc2adeb</t>
+          <t>ea987291874660999d0606ac6d0f6420</t>
         </is>
       </c>
       <c r="I43" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.bf9b7ebf564aef032fbf313ec38b8359cd0975b561fe1eb83577e50ed4dad1f6.5bba87e222^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.5d71177d4f1ca9c4f5aee2d6352a9c921d0dc1c2a00e9a75fe598c485e8677f3.2697b6a5d9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J43" s="68" t="inlineStr">
@@ -4714,22 +4714,22 @@
       </c>
       <c r="F44" s="67" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="G44" s="67" t="inlineStr">
         <is>
-          <t>2025-11-17T10:24:07Z</t>
+          <t>2025-11-20T09:36:16Z</t>
         </is>
       </c>
       <c r="H44" s="67" t="inlineStr">
         <is>
-          <t>263163f257a5f4099aa9a3858c98d3ba</t>
+          <t>fab53da6844bb7226854eca0d5695601</t>
         </is>
       </c>
       <c r="I44" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.07471ca25f4d8111dc8e683ddf0c6602ea6534203765060b5e2ea3b370aead44.cb126736e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.1be9811655cf330a12708a5e39b50224835da36261c5c7eb1dd53ed3641f1751.ca56e6793f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J44" s="68" t="inlineStr">

</xml_diff>

<commit_message>
Fix test OK LAB+RSA
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.56/report-checklist.xlsx
+++ b/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.56/report-checklist.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="33720" yWindow="975" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Istruzioni Compilazione" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Prerequisiti" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TestCases" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="LISTA VALORI" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="Summary" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Istruzioni Compilazione" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Prerequisiti" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TestCases" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LISTA VALORI" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'TestCases'!$A$9:$W$192</definedName>
@@ -2627,22 +2627,22 @@
       </c>
       <c r="F10" s="66" t="inlineStr">
         <is>
-          <t>2025-11-20</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="G10" s="66" t="inlineStr">
         <is>
-          <t>2025-11-20T09:36:13Z</t>
+          <t>2025-12-01T15:48:08Z</t>
         </is>
       </c>
       <c r="H10" s="66" t="inlineStr">
         <is>
-          <t>aa1e24be850220621e4bd400733d8957</t>
+          <t>79818d89a445489f04649241ac82b012</t>
         </is>
       </c>
       <c r="I10" s="67" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.206da0e5a5a596b3faa12030c1aef93330a218ee42be85a8a12e9f3ede6cf877.04aa7a6a73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.991b2f46f012d11ecce2a3c98c3b8cddd6e92248d48498fb57fcbe6d6476af85.86ca589fd1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J10" s="68" t="inlineStr">
@@ -2935,12 +2935,12 @@
       </c>
       <c r="F15" s="76" t="inlineStr">
         <is>
-          <t>2025-11-20</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="G15" s="76" t="inlineStr">
         <is>
-          <t>2025-11-20T09:37:19Z</t>
+          <t>2025-12-01T15:49:15Z</t>
         </is>
       </c>
       <c r="H15" s="76" t="inlineStr">
@@ -3035,12 +3035,12 @@
       </c>
       <c r="F16" s="76" t="inlineStr">
         <is>
-          <t>2025-11-20</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="G16" s="76" t="inlineStr">
         <is>
-          <t>2025-11-20T09:37:19Z</t>
+          <t>2025-12-01T15:49:15Z</t>
         </is>
       </c>
       <c r="H16" s="76" t="inlineStr">
@@ -4424,22 +4424,22 @@
       </c>
       <c r="F40" s="67" t="inlineStr">
         <is>
-          <t>2025-11-20</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="G40" s="67" t="inlineStr">
         <is>
-          <t>2025-11-20T09:36:20Z</t>
+          <t>2025-12-01T15:48:15Z</t>
         </is>
       </c>
       <c r="H40" s="67" t="inlineStr">
         <is>
-          <t>8564ac9347687d4a355e2dd0552e7004</t>
+          <t>a90ba88db63a4789ffd248b930f28f9e</t>
         </is>
       </c>
       <c r="I40" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.30406e6567059ad7e9e67de27e479b6fd3a38429dfe83af0291c3c6d34d86e0c.2d94ef14fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.7341a176d9d709f45692e3ea099f295bcee45a2a4a2a3f13b93df798b988d893.2ab7511711^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J40" s="68" t="inlineStr">
@@ -4497,22 +4497,22 @@
       </c>
       <c r="F41" s="67" t="inlineStr">
         <is>
-          <t>2025-11-20</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="G41" s="67" t="inlineStr">
         <is>
-          <t>2025-11-20T09:36:20Z</t>
+          <t>2025-12-01T15:48:16Z</t>
         </is>
       </c>
       <c r="H41" s="67" t="inlineStr">
         <is>
-          <t>192a9b156d7d54ec4cac6f58595967f6</t>
+          <t>e8b96a9c0100c9fe7b0b72c6dde4abdb</t>
         </is>
       </c>
       <c r="I41" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.208a06f1bb78b35c2631ad3d6bb87d030df622ece4aedc74ceabd822bf77e4a9.dee1dd0079^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.d518574401018b9d816884425ac5209b0f3d66624223a41e63e37c722a19097e.a885818bd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J41" s="68" t="inlineStr">
@@ -4569,22 +4569,22 @@
       </c>
       <c r="F42" s="67" t="inlineStr">
         <is>
-          <t>2025-11-20</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="G42" s="67" t="inlineStr">
         <is>
-          <t>2025-11-20T09:37:11Z</t>
+          <t>2025-12-01T15:49:07Z</t>
         </is>
       </c>
       <c r="H42" s="67" t="inlineStr">
         <is>
-          <t>9f8f2e4228bb8ed3a74164590e7b601f</t>
+          <t>bc1c5384309a3843895323d123d6c294</t>
         </is>
       </c>
       <c r="I42" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.c2135097a224aaaa6a9c09a5d4643ff57410e7a2761a60f422f5ad040f1b440b.37ff88e20b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.249ef45e6e6f9f83a0ced5415b6f41b8bed0fc1464d76543e871e9c1e115c63c.827ae37534^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J42" s="68" t="inlineStr">
@@ -4641,22 +4641,22 @@
       </c>
       <c r="F43" s="67" t="inlineStr">
         <is>
-          <t>2025-11-20</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="G43" s="67" t="inlineStr">
         <is>
-          <t>2025-11-20T09:37:15Z</t>
+          <t>2025-12-01T15:49:11Z</t>
         </is>
       </c>
       <c r="H43" s="67" t="inlineStr">
         <is>
-          <t>ea987291874660999d0606ac6d0f6420</t>
+          <t>b8ee7c882f18d92625e5e94962ef9f05</t>
         </is>
       </c>
       <c r="I43" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.5d71177d4f1ca9c4f5aee2d6352a9c921d0dc1c2a00e9a75fe598c485e8677f3.2697b6a5d9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.c8014a745f4d9f2546d9c51e82260cce0dbab98f07ffb26bdd252fc4fe55d705.3460ce9ae3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J43" s="68" t="inlineStr">
@@ -4714,22 +4714,22 @@
       </c>
       <c r="F44" s="67" t="inlineStr">
         <is>
-          <t>2025-11-20</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="G44" s="67" t="inlineStr">
         <is>
-          <t>2025-11-20T09:36:16Z</t>
+          <t>2025-12-01T15:48:12Z</t>
         </is>
       </c>
       <c r="H44" s="67" t="inlineStr">
         <is>
-          <t>fab53da6844bb7226854eca0d5695601</t>
+          <t>41af03925bb106213336f5e0c7d780c8</t>
         </is>
       </c>
       <c r="I44" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.1be9811655cf330a12708a5e39b50224835da36261c5c7eb1dd53ed3641f1751.ca56e6793f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.7bd3e0bf273306c12ff20b304ebdfa2b5612874d5e8bdb078a458013bc817d86.c1413c023a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J44" s="68" t="inlineStr">

</xml_diff>

<commit_message>
Fix test [376, 449]
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.56/report-checklist.xlsx
+++ b/GATEWAY/A1#111#POPPIXSRLXX/POPPIX_SRL/BEEBEEDOC/1.3.56/report-checklist.xlsx
@@ -2627,22 +2627,22 @@
       </c>
       <c r="F10" s="66" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="G10" s="66" t="inlineStr">
         <is>
-          <t>2025-12-01T15:48:08Z</t>
+          <t>2025-12-05T10:55:47Z</t>
         </is>
       </c>
       <c r="H10" s="66" t="inlineStr">
         <is>
-          <t>79818d89a445489f04649241ac82b012</t>
+          <t>6f6d4aa05ebd08dc37972a1d37b3edae</t>
         </is>
       </c>
       <c r="I10" s="67" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.991b2f46f012d11ecce2a3c98c3b8cddd6e92248d48498fb57fcbe6d6476af85.86ca589fd1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.76f42ee1d76717a25dd7500b628ddf95cd61e72d57b8610aa355da280d83d8cb.2cd97f9d8b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J10" s="68" t="inlineStr">
@@ -2935,12 +2935,12 @@
       </c>
       <c r="F15" s="76" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="G15" s="76" t="inlineStr">
         <is>
-          <t>2025-12-01T15:49:15Z</t>
+          <t>2025-12-05T10:56:54Z</t>
         </is>
       </c>
       <c r="H15" s="76" t="inlineStr">
@@ -3035,12 +3035,12 @@
       </c>
       <c r="F16" s="76" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="G16" s="76" t="inlineStr">
         <is>
-          <t>2025-12-01T15:49:15Z</t>
+          <t>2025-12-05T10:56:54Z</t>
         </is>
       </c>
       <c r="H16" s="76" t="inlineStr">
@@ -4424,22 +4424,22 @@
       </c>
       <c r="F40" s="67" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="G40" s="67" t="inlineStr">
         <is>
-          <t>2025-12-01T15:48:15Z</t>
+          <t>2025-12-05T10:55:54Z</t>
         </is>
       </c>
       <c r="H40" s="67" t="inlineStr">
         <is>
-          <t>a90ba88db63a4789ffd248b930f28f9e</t>
+          <t>e8a1529f3d0e943cdfd7163f15b61d38</t>
         </is>
       </c>
       <c r="I40" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.7341a176d9d709f45692e3ea099f295bcee45a2a4a2a3f13b93df798b988d893.2ab7511711^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.fea9ebdd6bebd9e89975792e4a9970cab429d9a8a60eb9cd8874efb3d51ced5f.f4d2d39f35^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J40" s="68" t="inlineStr">
@@ -4497,22 +4497,22 @@
       </c>
       <c r="F41" s="67" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="G41" s="67" t="inlineStr">
         <is>
-          <t>2025-12-01T15:48:16Z</t>
+          <t>2025-12-05T10:55:55Z</t>
         </is>
       </c>
       <c r="H41" s="67" t="inlineStr">
         <is>
-          <t>e8b96a9c0100c9fe7b0b72c6dde4abdb</t>
+          <t>df33c184d8fb57db29d287d3f21db66b</t>
         </is>
       </c>
       <c r="I41" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.d518574401018b9d816884425ac5209b0f3d66624223a41e63e37c722a19097e.a885818bd2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.64604bf7709d8a078d88fb0e093831baf53fa96c1a31ec9f24e2d2ef37ec0d3d.d6afd0146a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J41" s="68" t="inlineStr">
@@ -4569,22 +4569,22 @@
       </c>
       <c r="F42" s="67" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="G42" s="67" t="inlineStr">
         <is>
-          <t>2025-12-01T15:49:07Z</t>
+          <t>2025-12-05T10:56:47Z</t>
         </is>
       </c>
       <c r="H42" s="67" t="inlineStr">
         <is>
-          <t>bc1c5384309a3843895323d123d6c294</t>
+          <t>3aa4c200b4354305cb4b319ac9b01345</t>
         </is>
       </c>
       <c r="I42" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.249ef45e6e6f9f83a0ced5415b6f41b8bed0fc1464d76543e871e9c1e115c63c.827ae37534^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.c39433643216509903b93f0a5cfa21561397589ff20428ab17d2afb4ee3e3e6d.2cf20dc005^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J42" s="68" t="inlineStr">
@@ -4641,22 +4641,22 @@
       </c>
       <c r="F43" s="67" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="G43" s="67" t="inlineStr">
         <is>
-          <t>2025-12-01T15:49:11Z</t>
+          <t>2025-12-05T10:56:50Z</t>
         </is>
       </c>
       <c r="H43" s="67" t="inlineStr">
         <is>
-          <t>b8ee7c882f18d92625e5e94962ef9f05</t>
+          <t>f135342285012decee32f767b8886b3f</t>
         </is>
       </c>
       <c r="I43" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.c8014a745f4d9f2546d9c51e82260cce0dbab98f07ffb26bdd252fc4fe55d705.3460ce9ae3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.aaa4336c44663a268ba93a3f1b285266d427a087632d1959a639a030b760e0e6.e56a6e5c40^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J43" s="68" t="inlineStr">
@@ -4714,22 +4714,22 @@
       </c>
       <c r="F44" s="67" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-05</t>
         </is>
       </c>
       <c r="G44" s="67" t="inlineStr">
         <is>
-          <t>2025-12-01T15:48:12Z</t>
+          <t>2025-12-05T10:55:51Z</t>
         </is>
       </c>
       <c r="H44" s="67" t="inlineStr">
         <is>
-          <t>41af03925bb106213336f5e0c7d780c8</t>
+          <t>49d4552fcd38248833bfdd449fcd0e64</t>
         </is>
       </c>
       <c r="I44" s="81" t="inlineStr">
         <is>
-          <t>2.16.840.1.113883.2.9.2.120.4.4.7bd3e0bf273306c12ff20b304ebdfa2b5612874d5e8bdb078a458013bc817d86.c1413c023a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+          <t>2.16.840.1.113883.2.9.2.120.4.4.9460266cd2efe81ee6c48cd83c90a7d1c603815d3d99c6831ed8fa05b58a87b5.2382cf693f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
         </is>
       </c>
       <c r="J44" s="68" t="inlineStr">

</xml_diff>